<commit_message>
CDR Board Component Placement
Component placement on 50 mil grid.
</commit_message>
<xml_diff>
--- a/Data/bme688Data.xlsx
+++ b/Data/bme688Data.xlsx
@@ -8,46 +8,77 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akshat\Documents\GitHub\SDP-Team-31\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7066A884-A798-4097-9974-0EA0658D792B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DA2281-A5B7-4E66-BD26-0BC41ED9A704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>Temp Ref</t>
-  </si>
-  <si>
-    <t>Hum</t>
-  </si>
-  <si>
-    <t>Hum Ref</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>dTemp</t>
+  </si>
+  <si>
+    <t>dHum</t>
+  </si>
+  <si>
+    <t>Temp (*C)</t>
+  </si>
+  <si>
+    <t>Temp Ref (*C)</t>
+  </si>
+  <si>
+    <t>Hum (%)</t>
+  </si>
+  <si>
+    <t>Hum Ref (%)</t>
+  </si>
+  <si>
+    <t>Temp Accuracy</t>
+  </si>
+  <si>
+    <t>Hum Accuracy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,9 +106,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,223 +390,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>SUM(D6:D15)/10</f>
+        <v>0.33100000000000057</v>
+      </c>
+      <c r="G2">
+        <f>SUM(G6:G15)/10</f>
+        <v>1.0809999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0.88194444444444453</v>
-      </c>
-      <c r="B2">
-        <v>23.33</v>
-      </c>
-      <c r="C2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="B6">
+        <v>23.39</v>
+      </c>
+      <c r="C6">
         <v>23.1</v>
       </c>
-      <c r="D2">
-        <v>34.42</v>
-      </c>
-      <c r="E2">
+      <c r="D6">
+        <f t="shared" ref="D6:D15" si="0">ABS(B6-C6)</f>
+        <v>0.28999999999999915</v>
+      </c>
+      <c r="E6">
+        <v>34.35</v>
+      </c>
+      <c r="F6">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0.8833333333333333</v>
-      </c>
-      <c r="B3">
-        <v>23.39</v>
-      </c>
-      <c r="C3">
+      <c r="G6">
+        <f t="shared" ref="G6:G15" si="1">ABS(E6-F6)</f>
+        <v>0.64999999999999858</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.8847222222222223</v>
+      </c>
+      <c r="B7">
+        <v>23.4</v>
+      </c>
+      <c r="C7">
         <v>23.1</v>
       </c>
-      <c r="D3">
-        <v>34.35</v>
-      </c>
-      <c r="E3">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="E7">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="F7">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.8847222222222223</v>
-      </c>
-      <c r="B4">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.70000000000000284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="B8">
+        <v>23.44</v>
+      </c>
+      <c r="C8">
+        <v>23.1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="E8">
+        <v>34.270000000000003</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.72999999999999687</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.88750000000000007</v>
+      </c>
+      <c r="B9">
+        <v>23.47</v>
+      </c>
+      <c r="C9">
+        <v>23.6</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.13000000000000256</v>
+      </c>
+      <c r="E9">
+        <v>34.229999999999997</v>
+      </c>
+      <c r="F9">
+        <v>37</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>2.7700000000000031</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="B10">
+        <v>23.49</v>
+      </c>
+      <c r="C10">
+        <v>24.1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.61000000000000298</v>
+      </c>
+      <c r="E10">
+        <v>34.130000000000003</v>
+      </c>
+      <c r="F10">
+        <v>36</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1.8699999999999974</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.89027777777777783</v>
+      </c>
+      <c r="B11">
+        <v>23.52</v>
+      </c>
+      <c r="C11">
+        <v>24.3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.78000000000000114</v>
+      </c>
+      <c r="E11">
+        <v>34.14</v>
+      </c>
+      <c r="F11">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>2.8599999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.89166666666666661</v>
+      </c>
+      <c r="B12">
+        <v>23.7</v>
+      </c>
+      <c r="C12">
+        <v>24.1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.40000000000000213</v>
+      </c>
+      <c r="E12">
+        <v>34.08</v>
+      </c>
+      <c r="F12">
+        <v>34</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>7.9999999999998295E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.8930555555555556</v>
+      </c>
+      <c r="B13">
+        <v>23.62</v>
+      </c>
+      <c r="C13">
+        <v>23.8</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.17999999999999972</v>
+      </c>
+      <c r="E13">
+        <v>34.119999999999997</v>
+      </c>
+      <c r="F13">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.11999999999999744</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.89444444444444438</v>
+      </c>
+      <c r="B14">
+        <v>23.59</v>
+      </c>
+      <c r="C14">
+        <v>23.5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999858E-2</v>
+      </c>
+      <c r="E14">
+        <v>34.08</v>
+      </c>
+      <c r="F14">
+        <v>34</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>7.9999999999998295E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="B15">
+        <v>23.59</v>
+      </c>
+      <c r="C15">
         <v>23.4</v>
       </c>
-      <c r="C4">
-        <v>23.1</v>
-      </c>
-      <c r="D4">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="E4">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.19000000000000128</v>
+      </c>
+      <c r="E15">
+        <v>34.049999999999997</v>
+      </c>
+      <c r="F15">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.88611111111111107</v>
-      </c>
-      <c r="B5">
-        <v>23.44</v>
-      </c>
-      <c r="C5">
-        <v>23.1</v>
-      </c>
-      <c r="D5">
-        <v>34.270000000000003</v>
-      </c>
-      <c r="E5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.88750000000000007</v>
-      </c>
-      <c r="B6">
-        <v>23.47</v>
-      </c>
-      <c r="C6">
-        <v>23.6</v>
-      </c>
-      <c r="D6">
-        <v>34.229999999999997</v>
-      </c>
-      <c r="E6">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="B7">
-        <v>23.49</v>
-      </c>
-      <c r="C7">
-        <v>24.1</v>
-      </c>
-      <c r="D7">
-        <v>34.130000000000003</v>
-      </c>
-      <c r="E7">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.89027777777777783</v>
-      </c>
-      <c r="B8">
-        <v>23.52</v>
-      </c>
-      <c r="C8">
-        <v>24.3</v>
-      </c>
-      <c r="D8">
-        <v>34.14</v>
-      </c>
-      <c r="E8">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.89166666666666661</v>
-      </c>
-      <c r="B9">
-        <v>23.7</v>
-      </c>
-      <c r="C9">
-        <v>24.1</v>
-      </c>
-      <c r="D9">
-        <v>34.08</v>
-      </c>
-      <c r="E9">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.8930555555555556</v>
-      </c>
-      <c r="B10">
-        <v>23.62</v>
-      </c>
-      <c r="C10">
-        <v>23.8</v>
-      </c>
-      <c r="D10">
-        <v>34.119999999999997</v>
-      </c>
-      <c r="E10">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.89444444444444438</v>
-      </c>
-      <c r="B11">
-        <v>23.59</v>
-      </c>
-      <c r="C11">
-        <v>23.5</v>
-      </c>
-      <c r="D11">
-        <v>34.08</v>
-      </c>
-      <c r="E11">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="B12">
-        <v>23.59</v>
-      </c>
-      <c r="C12">
-        <v>23.4</v>
-      </c>
-      <c r="D12">
-        <v>34.049999999999997</v>
-      </c>
-      <c r="E12">
-        <v>35</v>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.95000000000000284</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>